<commit_message>
Update My english vocabulary.xlsx
add new words
</commit_message>
<xml_diff>
--- a/My english vocabulary.xlsx
+++ b/My english vocabulary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Gena\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Gena\Documents\GitHub\English\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22E59C-5F49-446D-A00A-1018B5E380DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2F0DE6-82C0-437B-8063-0092A9F987F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{9C0DBA5B-AABE-4FEA-9D40-AC7B434F2A93}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="323">
   <si>
     <t>to plug in</t>
   </si>
@@ -939,10 +940,61 @@
     <t>advance</t>
   </si>
   <si>
-    <t>продвижение</t>
-  </si>
-  <si>
     <t>продвижение, успех</t>
+  </si>
+  <si>
+    <t>liability</t>
+  </si>
+  <si>
+    <t>ответственность</t>
+  </si>
+  <si>
+    <t>do me a favor</t>
+  </si>
+  <si>
+    <t>you got to be kidding me</t>
+  </si>
+  <si>
+    <t>ты шутишь надо мной?</t>
+  </si>
+  <si>
+    <t>сделай мне одолжение, или услугу</t>
+  </si>
+  <si>
+    <t>rethink</t>
+  </si>
+  <si>
+    <t>передумать</t>
+  </si>
+  <si>
+    <t>can I look at it</t>
+  </si>
+  <si>
+    <t>могу я посмотреть на это?</t>
+  </si>
+  <si>
+    <t>what are you after</t>
+  </si>
+  <si>
+    <t>что ты хочешь,ищешь</t>
+  </si>
+  <si>
+    <t>Wacked</t>
+  </si>
+  <si>
+    <t>что-то странное</t>
+  </si>
+  <si>
+    <t>relentless</t>
+  </si>
+  <si>
+    <t>неустанный, непрекращающийся</t>
+  </si>
+  <si>
+    <t>map out</t>
+  </si>
+  <si>
+    <t>наметить</t>
   </si>
 </sst>
 </file>
@@ -1317,16 +1369,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89672B4-D95E-4F49-B4CD-006D68899548}">
-  <dimension ref="B2:D168"/>
+  <dimension ref="B2:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="D169" sqref="D169"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="37.5703125" style="1" customWidth="1"/>
   </cols>
@@ -2603,12 +2655,84 @@
         <v>302</v>
       </c>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" t="s">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
         <v>303</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="D169" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
         <v>305</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>307</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>308</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>311</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>313</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>315</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>317</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>319</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
+        <v>321</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>